<commit_message>
1. Fixed a bug when adding recipients in bulk, the system can now detect    emails in invalid format 2. Display error message to the Management GUI
</commit_message>
<xml_diff>
--- a/static/recipient_list/uploaded_recipients_info.xlsx
+++ b/static/recipient_list/uploaded_recipients_info.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Chenwei Niu\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62E2B973-F57D-458E-8C67-90214DC00028}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8980BE2-5422-458C-96B1-AB0B8AD012EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7080" yWindow="4750" windowWidth="27260" windowHeight="15760" xr2:uid="{73713144-1402-437F-B68E-793AB810BF78}"/>
+    <workbookView xWindow="1120" yWindow="1780" windowWidth="27260" windowHeight="15760" xr2:uid="{73713144-1402-437F-B68E-793AB810BF78}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>name</t>
   </si>
@@ -54,9 +54,6 @@
   </si>
   <si>
     <t>anu</t>
-  </si>
-  <si>
-    <t>2@2</t>
   </si>
   <si>
     <t>unimelb</t>
@@ -447,7 +444,7 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.25"/>
@@ -482,17 +479,20 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B3" s="1" t="s">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1">
+        <v>222</v>
+      </c>
+      <c r="D3" t="s">
         <v>6</v>
-      </c>
-      <c r="D3" t="s">
-        <v>7</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" xr:uid="{DB6AADB3-C1F2-4C62-B9EF-9D424EBC677D}"/>
-    <hyperlink ref="B3" r:id="rId2" xr:uid="{110F38B8-5DA2-4E08-8BD0-7B810408EF97}"/>
+    <hyperlink ref="B3" r:id="rId2" display="2@2" xr:uid="{110F38B8-5DA2-4E08-8BD0-7B810408EF97}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
fixed padding bug in HTML template
</commit_message>
<xml_diff>
--- a/static/recipient_list/uploaded_recipients_info.xlsx
+++ b/static/recipient_list/uploaded_recipients_info.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Chenwei Niu\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8980BE2-5422-458C-96B1-AB0B8AD012EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2536DC99-B0DA-42D7-9632-4878A15D9DC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1120" yWindow="1780" windowWidth="27260" windowHeight="15760" xr2:uid="{73713144-1402-437F-B68E-793AB810BF78}"/>
+    <workbookView xWindow="13390" yWindow="5090" windowWidth="27260" windowHeight="14930" xr2:uid="{73713144-1402-437F-B68E-793AB810BF78}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>name</t>
   </si>
@@ -54,6 +54,9 @@
   </si>
   <si>
     <t>anu</t>
+  </si>
+  <si>
+    <t>2@2</t>
   </si>
   <si>
     <t>unimelb</t>
@@ -443,8 +446,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B2EB508-11A8-4BDD-B338-11EAA72EF4F4}">
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView tabSelected="1" zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.25"/>
@@ -482,17 +485,17 @@
       <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3" s="1">
-        <v>222</v>
+      <c r="B3" s="1" t="s">
+        <v>6</v>
       </c>
       <c r="D3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" xr:uid="{DB6AADB3-C1F2-4C62-B9EF-9D424EBC677D}"/>
-    <hyperlink ref="B3" r:id="rId2" display="2@2" xr:uid="{110F38B8-5DA2-4E08-8BD0-7B810408EF97}"/>
+    <hyperlink ref="B3" r:id="rId2" xr:uid="{110F38B8-5DA2-4E08-8BD0-7B810408EF97}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>